<commit_message>
first server side push
</commit_message>
<xml_diff>
--- a/server/initialdata/测试数据.xlsx
+++ b/server/initialdata/测试数据.xlsx
@@ -11,12 +11,12 @@
     <sheet name="导师" sheetId="2" r:id="rId2"/>
     <sheet name="课题" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
   <si>
     <t>学号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,22 +220,10 @@
     <t>云计算</t>
   </si>
   <si>
-    <t>云计算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人工智能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>图形图像处理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>多媒体</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>图形图像处理，程序语言</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -362,6 +350,61 @@
   </si>
   <si>
     <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技艺占比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盛新怡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人机交互</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>律睿敏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>互动媒体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人工智能,信息安全</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多媒体,其它</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>云计算,其它,web</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自我介绍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我是王明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我是李红</t>
+  </si>
+  <si>
+    <t>gpa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,11 +448,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -714,19 +758,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,8 +784,14 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1030513401</v>
       </c>
@@ -753,8 +804,14 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" s="2">
+        <v>3.21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1030513402</v>
       </c>
@@ -767,8 +824,14 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1030513403</v>
       </c>
@@ -781,8 +844,14 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1030513404</v>
       </c>
@@ -795,8 +864,14 @@
       <c r="D5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E5" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1030513405</v>
       </c>
@@ -809,8 +884,14 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E6" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1030513406</v>
       </c>
@@ -823,8 +904,14 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E7" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1030513407</v>
       </c>
@@ -837,8 +924,14 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E8" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1030513408</v>
       </c>
@@ -851,8 +944,14 @@
       <c r="D9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E9" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1030513409</v>
       </c>
@@ -865,8 +964,14 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E10" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1030513410</v>
       </c>
@@ -879,8 +984,14 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E11" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1030513411</v>
       </c>
@@ -893,8 +1004,14 @@
       <c r="D12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E12" s="2">
+        <v>3.43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1030513412</v>
       </c>
@@ -907,8 +1024,14 @@
       <c r="D13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E13" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1030513413</v>
       </c>
@@ -921,8 +1044,14 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E14" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1030513414</v>
       </c>
@@ -935,8 +1064,14 @@
       <c r="D15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E15" s="2">
+        <v>3.35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1030513415</v>
       </c>
@@ -949,8 +1084,14 @@
       <c r="D16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E16" s="2">
+        <v>3.36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1030513416</v>
       </c>
@@ -963,8 +1104,14 @@
       <c r="D17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E17" s="2">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>1030513417</v>
       </c>
@@ -977,8 +1124,14 @@
       <c r="D18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E18" s="2">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>1030513418</v>
       </c>
@@ -991,8 +1144,14 @@
       <c r="D19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E19" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>1030513419</v>
       </c>
@@ -1004,6 +1163,12 @@
       </c>
       <c r="D20" t="s">
         <v>30</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2.04</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1015,19 +1180,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1038,197 +1204,273 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>1030113001</v>
+        <v>2030513401</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
       <c r="C2">
-        <v>1030113001</v>
+        <v>2030513401</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>1030113002</v>
+        <v>2030513402</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
       <c r="C3">
-        <v>1030113002</v>
+        <v>2030513402</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>1030113003</v>
+        <v>2030513403</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
       </c>
       <c r="C4">
-        <v>1030113003</v>
+        <v>2030513403</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+      <c r="F4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>1030113004</v>
+        <v>2030513404</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5">
-        <v>1030113004</v>
+        <v>2030513404</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+      <c r="F5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>1030113005</v>
+        <v>2030513405</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
       </c>
       <c r="C6">
-        <v>1030113005</v>
+        <v>2030513405</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+      <c r="F6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>1030113006</v>
+        <v>2030513406</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
       <c r="C7">
-        <v>1030113006</v>
+        <v>2030513406</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+      <c r="F7">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>1030113007</v>
+        <v>2030513407</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
       <c r="C8">
-        <v>1030113007</v>
+        <v>2030513407</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>1030113008</v>
+        <v>2030513408</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
       </c>
       <c r="C9">
-        <v>1030113008</v>
+        <v>2030513408</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>96</v>
+      </c>
+      <c r="F9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>1030113009</v>
+        <v>2030513409</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
       </c>
       <c r="C10">
-        <v>1030113009</v>
+        <v>2030513409</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2030513410</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>2030513410</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2030513411</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>2030513411</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>1030113010</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11">
-        <v>1030113010</v>
-      </c>
-      <c r="D11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12">
-        <v>1030113011</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12">
-        <v>1030113011</v>
-      </c>
-      <c r="D12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" t="s">
-        <v>59</v>
+      <c r="F12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2030513412</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>2030513412</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2030513413</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14">
+        <v>2030513413</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1254,22 +1496,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -1277,10 +1519,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1289,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -1297,10 +1539,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1309,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -1317,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1337,10 +1579,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1349,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27" x14ac:dyDescent="0.15">
@@ -1357,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1377,10 +1619,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1389,7 +1631,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>